<commit_message>
Change Excell sheet name from "Standardized Mean Diff Final" to "Standardized Mean Diff"
</commit_message>
<xml_diff>
--- a/AlzheimersData.xlsx
+++ b/AlzheimersData.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tamara.vrublevskaya\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonid\Dev\ma_in_r\ma_in_r\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E410D5A3-609C-4CEC-B331-25213EF53EF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0622F3-3FB4-41E9-AAD3-AF174B20A1CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="901" xr2:uid="{ADE7099F-610E-4887-9F05-5E495A850C05}"/>
+    <workbookView xWindow="3135" yWindow="1215" windowWidth="28800" windowHeight="17085" tabRatio="901" activeTab="2" xr2:uid="{ADE7099F-610E-4887-9F05-5E495A850C05}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Standardized Mean Diff" sheetId="1" r:id="rId1"/>
-    <sheet name="Standardized Mean Diff Final" sheetId="7" r:id="rId2"/>
+    <sheet name="Standardized Mean Diff" sheetId="7" r:id="rId2"/>
     <sheet name="Combined Groups Analysis" sheetId="8" r:id="rId3"/>
     <sheet name="Excluded Standardized Mean Diff" sheetId="3" r:id="rId4"/>
     <sheet name="Need to Derive Mean Diff" sheetId="4" r:id="rId5"/>
@@ -2924,7 +2924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0B70213-206F-4D11-882C-9E169C63C1C6}">
   <dimension ref="A1:AF213"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -27058,7 +27058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A5B80F6-D9F3-4ECA-A895-DB8F584AB6C0}">
   <dimension ref="A1:S108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="B56" sqref="B56:B109"/>

</xml_diff>